<commit_message>
progress on dev spreadsheet
</commit_message>
<xml_diff>
--- a/MFET0450/project2/development_spreadsheet.xlsx
+++ b/MFET0450/project2/development_spreadsheet.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profiles\mtl9706\github\EleventhSemester\MFET0450\project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0E0C67FA-C633-408A-BB83-F7D57FC91E72}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF1BF94-BD88-4C26-9158-891C451C8139}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Laurentys_Matheus_Program-Tags" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="202">
   <si>
     <t>DATATYPE</t>
   </si>
@@ -547,22 +547,91 @@
     <t>| FEEDER | - Total volume the conveyor needs to fill the bottles</t>
   </si>
   <si>
-    <t>| CONVEYOR | -</t>
-  </si>
-  <si>
     <t>| FEEDER | - Indicates bottles is liquid minimum threshold is reached</t>
   </si>
   <si>
     <t>| PACKAGING | -</t>
   </si>
   <si>
-    <t xml:space="preserve">| CONVEYOR | - </t>
+    <t>| CONVEYOR | - Whether the amount of bottles requested were filled</t>
+  </si>
+  <si>
+    <t>| CONVEYOR | - Whether the feeder is ready for the system to startup</t>
+  </si>
+  <si>
+    <t>| CONVEYOR | - Whether the bottle requested from the feeder is in the conveyor</t>
+  </si>
+  <si>
+    <t>| FEEDER | - Unused variable but required by the SBR tag</t>
+  </si>
+  <si>
+    <t>| CONVEYOR | - Unused variable but required by the SBR tag</t>
+  </si>
+  <si>
+    <t>| PACKAGING | - Unused variable but required by the SBR tag</t>
+  </si>
+  <si>
+    <t>| CONVEYOR | - Whether the shutdown system is running</t>
+  </si>
+  <si>
+    <t>| CONVEYOR | - Whether the recovery system is running</t>
+  </si>
+  <si>
+    <t>| CONVEYOR | - Whether the conveyor is powered on</t>
+  </si>
+  <si>
+    <t>| CONVEYOR | - Number of bottles in the conveyor</t>
+  </si>
+  <si>
+    <t>| CONVEYOR | - Number of bottles trying to be filled</t>
+  </si>
+  <si>
+    <t>| CONVEYOR | - Timer used to simulate system shutdown and recovery</t>
+  </si>
+  <si>
+    <t>| PACKAGING | - Whether the current number of bottles were filled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">| PACKAGING | - ONS used to simulate subsystem packing specific bottles </t>
+  </si>
+  <si>
+    <t>| PACKAGING | - Whether the main system is running</t>
+  </si>
+  <si>
+    <t>| PACKAGING | - Number of bottles trying to be filled</t>
+  </si>
+  <si>
+    <t>| PACKAGING | - Number of packed boxes of type 0 with liquid 0</t>
+  </si>
+  <si>
+    <t>| PACKAGING | - Number of packed boxes of type 0 with liquid 1</t>
+  </si>
+  <si>
+    <t>| PACKAGING | - Number of packed boxes of type 1 with liquid 0</t>
+  </si>
+  <si>
+    <t>| PACKAGING | - Number of packed boxes of type 1 with liquid 1</t>
+  </si>
+  <si>
+    <t>| PACKAGING | - Number of bottles of type 0 with liquid 0 ready to be packed</t>
+  </si>
+  <si>
+    <t>| PACKAGING | - Number of bottles of type 0 with liquid 1 ready to be packed</t>
+  </si>
+  <si>
+    <t>| PACKAGING | - Number of bottles of type 1 with liquid 0 ready to be packed</t>
+  </si>
+  <si>
+    <t>| PACKAGING | - Number of bottles of type 1 with liquid 1 ready to be packed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">| PACKAGING | - </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1399,16 +1468,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="71.140625" customWidth="1"/>
+    <col min="3" max="3" width="72.7109375" customWidth="1"/>
     <col min="4" max="4" width="38" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" customWidth="1"/>
@@ -2146,10 +2215,10 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D40" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="F40" t="s">
         <v>3</v>
@@ -2160,10 +2229,10 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="D41" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="F41" t="s">
         <v>3</v>
@@ -2174,10 +2243,10 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D42" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="F42" t="s">
         <v>3</v>
@@ -2188,10 +2257,10 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D43" t="s">
-        <v>101</v>
+        <v>39</v>
       </c>
       <c r="F43" t="s">
         <v>3</v>
@@ -2202,13 +2271,13 @@
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D44" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="F44" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
@@ -2216,13 +2285,13 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="D45" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="F45" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
@@ -2230,10 +2299,10 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D46" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="F46" t="s">
         <v>7</v>
@@ -2244,10 +2313,10 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D47" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="F47" t="s">
         <v>7</v>
@@ -2258,10 +2327,10 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D48" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F48" t="s">
         <v>7</v>
@@ -2272,10 +2341,10 @@
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D49" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F49" t="s">
         <v>7</v>
@@ -2286,10 +2355,10 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F50" t="s">
         <v>7</v>
@@ -2300,10 +2369,10 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D51" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
       <c r="F51" t="s">
         <v>7</v>
@@ -2314,10 +2383,10 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D52" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="F52" t="s">
         <v>7</v>
@@ -2328,10 +2397,10 @@
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D53" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="F53" t="s">
         <v>7</v>
@@ -2342,13 +2411,13 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D54" t="s">
-        <v>2</v>
+        <v>106</v>
       </c>
       <c r="F54" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
@@ -2356,10 +2425,10 @@
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D55" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="F55" t="s">
         <v>3</v>
@@ -2370,10 +2439,10 @@
         <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D56" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="F56" t="s">
         <v>3</v>
@@ -2384,10 +2453,10 @@
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D57" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="F57" t="s">
         <v>3</v>
@@ -2398,10 +2467,10 @@
         <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="D58" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F58" t="s">
         <v>3</v>
@@ -2412,10 +2481,10 @@
         <v>1</v>
       </c>
       <c r="C59" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="D59" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F59" t="s">
         <v>3</v>
@@ -2426,10 +2495,10 @@
         <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="D60" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F60" t="s">
         <v>3</v>
@@ -2440,13 +2509,13 @@
         <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="D61" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
       <c r="F61" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
@@ -2454,13 +2523,13 @@
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="D62" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F62" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.25">
@@ -2468,13 +2537,13 @@
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="D63" t="s">
-        <v>79</v>
+        <v>6</v>
       </c>
       <c r="F63" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.25">
@@ -2482,13 +2551,13 @@
         <v>1</v>
       </c>
       <c r="C64" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="D64" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="F64" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
@@ -2496,10 +2565,10 @@
         <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="D65" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F65" t="s">
         <v>3</v>
@@ -2510,10 +2579,10 @@
         <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="D66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F66" t="s">
         <v>3</v>
@@ -2524,10 +2593,10 @@
         <v>1</v>
       </c>
       <c r="C67" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="D67" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F67" t="s">
         <v>3</v>
@@ -2538,10 +2607,10 @@
         <v>1</v>
       </c>
       <c r="C68" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="D68" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F68" t="s">
         <v>3</v>
@@ -2552,10 +2621,10 @@
         <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="D69" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="F69" t="s">
         <v>3</v>
@@ -2566,10 +2635,10 @@
         <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="D70" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="F70" t="s">
         <v>3</v>
@@ -2580,7 +2649,7 @@
         <v>1</v>
       </c>
       <c r="C71" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="D71" t="s">
         <v>82</v>
@@ -2594,7 +2663,7 @@
         <v>1</v>
       </c>
       <c r="C72" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="D72" t="s">
         <v>13</v>
@@ -2608,7 +2677,7 @@
         <v>1</v>
       </c>
       <c r="C73" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="D73" t="s">
         <v>14</v>
@@ -2622,7 +2691,7 @@
         <v>1</v>
       </c>
       <c r="C74" t="s">
-        <v>177</v>
+        <v>195</v>
       </c>
       <c r="D74" t="s">
         <v>15</v>
@@ -2636,7 +2705,7 @@
         <v>1</v>
       </c>
       <c r="C75" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
       <c r="D75" t="s">
         <v>16</v>
@@ -2650,7 +2719,7 @@
         <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="D76" t="s">
         <v>8</v>
@@ -2664,7 +2733,7 @@
         <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="D77" t="s">
         <v>102</v>
@@ -2678,7 +2747,7 @@
         <v>1</v>
       </c>
       <c r="C78" t="s">
-        <v>177</v>
+        <v>198</v>
       </c>
       <c r="D78" t="s">
         <v>103</v>
@@ -2692,7 +2761,7 @@
         <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>177</v>
+        <v>199</v>
       </c>
       <c r="D79" t="s">
         <v>104</v>
@@ -2706,7 +2775,7 @@
         <v>1</v>
       </c>
       <c r="C80" t="s">
-        <v>177</v>
+        <v>200</v>
       </c>
       <c r="D80" t="s">
         <v>105</v>
@@ -2720,7 +2789,7 @@
         <v>1</v>
       </c>
       <c r="C81" t="s">
-        <v>177</v>
+        <v>201</v>
       </c>
       <c r="D81" t="s">
         <v>40</v>
@@ -2734,7 +2803,7 @@
         <v>1</v>
       </c>
       <c r="C82" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D82" t="s">
         <v>62</v>

</xml_diff>